<commit_message>
better labels in Excel Templates
</commit_message>
<xml_diff>
--- a/TestTDMS/Result_Collection--MST2022081100.xlsx
+++ b/TestTDMS/Result_Collection--MST2022081100.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ven-file\data1\ENTWICKLUNG\Software\data_automator\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ven-file\data1\ENTWICKLUNG\Software\data_automator\TestTDMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23434330-A5B7-46DB-8919-B55E0C5D0D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124BAF19-B79A-4B81-8C96-76862DF62A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Maximum</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>F:/ENTWICKLUNG/Software/data_automator/Test/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_004_24V_20230228_110311.xlsx</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -66,58 +63,70 @@
     <t>12V F2-F3</t>
   </si>
   <si>
-    <t>LLP Zeit</t>
-  </si>
-  <si>
-    <t>LLP Strom avg</t>
-  </si>
-  <si>
-    <t>LLP Strom avg MAX 100ms</t>
-  </si>
-  <si>
-    <t>LLP Drehzahl avg</t>
-  </si>
-  <si>
-    <t>LLP Hübe</t>
-  </si>
-  <si>
-    <t>Lastpunkt</t>
-  </si>
-  <si>
-    <t>Drehzahl bei I_nenn</t>
-  </si>
-  <si>
-    <t>max avg 20ms:</t>
-  </si>
-  <si>
-    <t>max avg 40ms:</t>
-  </si>
-  <si>
-    <t>max avg 150ms:</t>
-  </si>
-  <si>
-    <t>max avg 750ms:</t>
-  </si>
-  <si>
-    <t>Tstart Zyl</t>
-  </si>
-  <si>
-    <t>Tmax Zyl</t>
-  </si>
-  <si>
-    <t>Tavg Zyl</t>
-  </si>
-  <si>
-    <t>Tstart Motor</t>
-  </si>
-  <si>
-    <t>Tmax Motor</t>
-  </si>
-  <si>
-    <t>F:/ENTWICKLUNG/Software/data_automator/Test/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_005_24V_20230228_114323.xlsx</t>
+    <t>Strom Limit [A]</t>
+  </si>
+  <si>
+    <t>Wird Strom überschritten? (1..Ja, 0..Nein)</t>
+  </si>
+  <si>
+    <t>(LLP Strom avg MAX 100ms) - (Strom Limit)  [A]</t>
+  </si>
+  <si>
+    <t>LLP Zeit [ms]</t>
+  </si>
+  <si>
+    <t>LLP Strom avg [A]</t>
+  </si>
+  <si>
+    <t>LLP Strom avg MAX 100ms [A]</t>
+  </si>
+  <si>
+    <t>LLP Drehzahl avg [1]</t>
+  </si>
+  <si>
+    <t>LLP Hübe (berechnet aus durchschn. Drehzahl) [A]</t>
+  </si>
+  <si>
+    <t>Durchschn. Strom zwischen 7 und 8 bar (Lastpunkt) [A]</t>
+  </si>
+  <si>
+    <t>Drehzahl bei I_nenn=8 A [RPM]</t>
+  </si>
+  <si>
+    <t>Strom max avg 20ms [A]</t>
+  </si>
+  <si>
+    <t>Strom max avg 40ms [A]</t>
+  </si>
+  <si>
+    <t>Strom max avg 150ms [A]</t>
+  </si>
+  <si>
+    <t>Strom max avg 750ms [A]</t>
+  </si>
+  <si>
+    <t>Tstart Zyl [°C]</t>
+  </si>
+  <si>
+    <t>Tmax Zyl  [°C]</t>
+  </si>
+  <si>
+    <t>Tavg Zyl  [°C]</t>
+  </si>
+  <si>
+    <t>Tstart Motor  [°C]</t>
+  </si>
+  <si>
+    <t>Tmax Motor  [°C]</t>
+  </si>
+  <si>
+    <t>F:/ENTWICKLUNG/Software/data_automator/TestTDMS/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_004_24V_20230228_110311.xlsx</t>
   </si>
   <si>
     <t>CSI_FKT 1 F2-F3 1 MST2022081100_005_24V_20230228_114323</t>
+  </si>
+  <si>
+    <t>F:/ENTWICKLUNG/Software/data_automator/TestTDMS/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_005_24V_20230228_114323.xlsx</t>
   </si>
 </sst>
 </file>
@@ -162,11 +171,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -451,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:E22"/>
+  <dimension ref="A3:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -459,223 +465,236 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>-4.1756250000000001</v>
+      </c>
+      <c r="G4">
+        <v>62.451000000000001</v>
+      </c>
+      <c r="H4">
+        <v>4.1086501933484918</v>
+      </c>
+      <c r="I4">
+        <v>4.8243749999999999</v>
+      </c>
+      <c r="J4">
+        <v>5872.0469820822391</v>
+      </c>
+      <c r="K4">
+        <v>6111.9201013002985</v>
+      </c>
+      <c r="L4">
+        <v>4.2879709135047657</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>13.391406249999999</v>
+      </c>
+      <c r="O4">
+        <v>9.6988281250000004</v>
+      </c>
+      <c r="P4">
+        <v>5.8767708333333335</v>
+      </c>
+      <c r="Q4">
+        <v>4.6466041666666671</v>
+      </c>
+      <c r="R4">
+        <v>21.793118</v>
+      </c>
+      <c r="S4">
+        <v>83.742676000000003</v>
+      </c>
+      <c r="T4">
+        <v>54.769798038461524</v>
+      </c>
+      <c r="U4">
+        <v>21.789793</v>
+      </c>
+      <c r="V4">
+        <v>25.609445999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="D5">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
-        <v>62.451000000000001</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>-4.3092187500000003</v>
+      </c>
+      <c r="G5">
         <v>62.722999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4.1086501933484918</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="H5">
         <v>3.9921424115968369</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4.8243749999999999</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="I5">
         <v>4.6907812499999997</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1">
-        <v>5872.0469820822391</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="J5">
         <v>5861.1130209329758</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6111.9201013002985</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="K5">
         <v>6127.1098668663171</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4.2879709135047657</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="L5">
         <v>4.2101003475912151</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1">
-        <v>13.391406249999999</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>13.34765625</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1">
-        <v>9.6988281250000004</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="O5">
         <v>9.580078125</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5.8767708333333335</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="P5">
         <v>5.6693749999999996</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1">
-        <v>4.6466041666666671</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="Q5">
         <v>4.4997291666666666</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="1">
-        <v>21.793118</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="R5">
         <v>21.722351</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="1">
-        <v>83.742676000000003</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="S5">
         <v>92.511110000000002</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="1">
-        <v>54.769798038461524</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="T5">
         <v>58.910318696202552</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="1">
-        <v>21.789793</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="U5">
         <v>21.789964999999999</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="1">
-        <v>25.609445999999998</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="V5">
         <v>25.616503000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" tooltip="F:/ENTWICKLUNG/Software/data_automator/Test/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_004_24V_20230228_110311.xlsx - Click once to follow. Click and hold to select this cell." xr:uid="{59A26B02-2643-4CEE-B799-9F85273E97BA}"/>
-    <hyperlink ref="E4" r:id="rId2" tooltip="F:/ENTWICKLUNG/Software/data_automator/Test/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_005_24V_20230228_114323.xlsx - Click once to follow. Click and hold to select this cell." xr:uid="{8E18ABA1-587B-4B0F-AC5C-37B5ED0EDA9F}"/>
+    <hyperlink ref="A4" r:id="rId1" tooltip="F:/ENTWICKLUNG/Software/data_automator/TestTDMS/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_004_24V_20230228_110311.xlsx - Click once to follow. Click and hold to select this cell." xr:uid="{B4CE0518-15AD-478F-ABCD-522AE155C429}"/>
+    <hyperlink ref="A5" r:id="rId2" tooltip="F:/ENTWICKLUNG/Software/data_automator/TestTDMS/12V F2-F3--CSI_FKT 1 F2-F3 1 MST2022081100_005_24V_20230228_114323.xlsx - Click once to follow. Click and hold to select this cell." xr:uid="{62228F76-2448-4244-B514-13346EE9D7A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -711,9 +730,9 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="str">
+      <c r="B6">
         <f>Result!C6</f>
-        <v>TestName</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>MAX(Result!D6:BZ6)</f>
@@ -729,117 +748,117 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="str">
+      <c r="B7">
         <f>Result!C7</f>
-        <v>LLP Zeit</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>MAX(Result!D7:BZ7)</f>
-        <v>62.722999999999999</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f>MIN(Result!D7:BZ7)</f>
-        <v>62.451000000000001</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E24" si="0">C7-D7</f>
-        <v>0.27199999999999847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="str">
+      <c r="B8">
         <f>Result!C8</f>
-        <v>LLP Strom avg</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>MAX(Result!D8:BZ8)</f>
-        <v>4.1086501933484918</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>MIN(Result!D8:BZ8)</f>
-        <v>3.9921424115968369</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.11650778175165488</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="str">
+      <c r="B9">
         <f>Result!C9</f>
-        <v>LLP Strom avg MAX 100ms</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f>MAX(Result!D9:BZ9)</f>
-        <v>4.8243749999999999</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f>MIN(Result!D9:BZ9)</f>
-        <v>4.6907812499999997</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.13359375000000018</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="str">
+      <c r="B10">
         <f>Result!C10</f>
-        <v>LLP Drehzahl avg</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f>MAX(Result!D10:BZ10)</f>
-        <v>5872.0469820822391</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f>MIN(Result!D10:BZ10)</f>
-        <v>5861.1130209329758</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>10.933961149263268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="str">
+      <c r="B11">
         <f>Result!C11</f>
-        <v>LLP Hübe</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <f>MAX(Result!D11:BZ11)</f>
-        <v>6127.1098668663171</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f>MIN(Result!D11:BZ11)</f>
-        <v>6111.9201013002985</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>15.18976556601865</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
+      <c r="B12">
         <f>Result!C12</f>
-        <v>Lastpunkt</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f>MAX(Result!D12:BZ12)</f>
-        <v>4.2879709135047657</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f>MIN(Result!D12:BZ12)</f>
-        <v>4.2101003475912151</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>7.7870565913550571E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
+      <c r="B13">
         <f>Result!C13</f>
-        <v>Drehzahl bei I_nenn</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <f>MAX(Result!D13:BZ13)</f>
@@ -855,165 +874,165 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="str">
+      <c r="B14">
         <f>Result!C14</f>
-        <v>max avg 20ms:</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <f>MAX(Result!D14:BZ14)</f>
-        <v>13.391406249999999</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f>MIN(Result!D14:BZ14)</f>
-        <v>13.34765625</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>4.3749999999999289E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="str">
+      <c r="B15">
         <f>Result!C15</f>
-        <v>max avg 40ms:</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <f>MAX(Result!D15:BZ15)</f>
-        <v>9.6988281250000004</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f>MIN(Result!D15:BZ15)</f>
-        <v>9.580078125</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.11875000000000036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="str">
+      <c r="B16">
         <f>Result!C16</f>
-        <v>max avg 150ms:</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <f>MAX(Result!D16:BZ16)</f>
-        <v>5.8767708333333335</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <f>MIN(Result!D16:BZ16)</f>
-        <v>5.6693749999999996</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.20739583333333389</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="str">
+      <c r="B17">
         <f>Result!C17</f>
-        <v>max avg 750ms:</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <f>MAX(Result!D17:BZ17)</f>
-        <v>4.6466041666666671</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <f>MIN(Result!D17:BZ17)</f>
-        <v>4.4997291666666666</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.14687500000000053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="str">
+      <c r="B18">
         <f>Result!C18</f>
-        <v>Tstart Zyl</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <f>MAX(Result!D18:BZ18)</f>
-        <v>21.793118</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <f>MIN(Result!D18:BZ18)</f>
-        <v>21.722351</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>7.0767000000000024E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="str">
+      <c r="B19">
         <f>Result!C19</f>
-        <v>Tmax Zyl</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <f>MAX(Result!D19:BZ19)</f>
-        <v>92.511110000000002</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <f>MIN(Result!D19:BZ19)</f>
-        <v>83.742676000000003</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>8.7684339999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="str">
+      <c r="B20">
         <f>Result!C20</f>
-        <v>Tavg Zyl</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <f>MAX(Result!D20:BZ20)</f>
-        <v>58.910318696202552</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <f>MIN(Result!D20:BZ20)</f>
-        <v>54.769798038461524</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>4.1405206577410283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+      <c r="B21">
         <f>Result!C21</f>
-        <v>Tstart Motor</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <f>MAX(Result!D21:BZ21)</f>
-        <v>21.789964999999999</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <f>MIN(Result!D21:BZ21)</f>
-        <v>21.789793</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1.7199999999917281E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
+      <c r="B22">
         <f>Result!C22</f>
-        <v>Tmax Motor</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <f>MAX(Result!D22:BZ22)</f>
-        <v>25.616503000000002</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <f>MIN(Result!D22:BZ22)</f>
-        <v>25.609445999999998</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>7.0570000000031996E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>